<commit_message>
ALPHA - Export functionality added
</commit_message>
<xml_diff>
--- a/NTDS_Amsterdam.xlsx
+++ b/NTDS_Amsterdam.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14400" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="15000" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="164">
   <si>
-    <t>Breiten</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Nummer</t>
   </si>
   <si>
@@ -62,9 +56,6 @@
     <t>Team-captain</t>
   </si>
   <si>
-    <t>Beginner</t>
-  </si>
-  <si>
     <t>EHBO</t>
   </si>
   <si>
@@ -516,6 +507,15 @@
   </si>
   <si>
     <t>Rene</t>
+  </si>
+  <si>
+    <t>Breitensport</t>
+  </si>
+  <si>
+    <t>Beginners</t>
+  </si>
+  <si>
+    <t>Open Class</t>
   </si>
 </sst>
 </file>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +892,8 @@
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
@@ -912,73 +913,73 @@
   <sheetData>
     <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -986,42 +987,42 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M2" s="2"/>
       <c r="O2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="S2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1029,42 +1030,42 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M3" s="2"/>
       <c r="O3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -1072,22 +1073,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H4" s="2">
         <v>8</v>
@@ -1096,17 +1097,17 @@
         <v>8</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="2"/>
       <c r="O4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="S4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -1117,42 +1118,42 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="O5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="S5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1160,22 +1161,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H6" s="2">
         <v>36</v>
@@ -1184,22 +1185,22 @@
         <v>36</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="O6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="S6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1207,49 +1208,49 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M7" s="2"/>
       <c r="O7" s="2"/>
       <c r="Q7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1257,20 +1258,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H8" s="2">
         <v>14</v>
@@ -1279,10 +1280,10 @@
         <v>14</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1290,11 +1291,11 @@
       <c r="Q8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1302,20 +1303,20 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H9" s="2">
         <v>3</v>
@@ -1324,17 +1325,17 @@
         <v>3</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="O9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="S9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -1345,30 +1346,30 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1377,7 +1378,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V10" s="2"/>
     </row>
@@ -1386,42 +1387,42 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M11" s="2"/>
       <c r="O11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1429,47 +1430,47 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M12" s="2"/>
       <c r="O12" s="2"/>
       <c r="Q12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1477,20 +1478,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H13" s="2">
         <v>18</v>
@@ -1499,10 +1500,10 @@
         <v>18</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1510,11 +1511,11 @@
       <c r="Q13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U13" s="2"/>
       <c r="V13" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1522,41 +1523,41 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M14" s="2"/>
       <c r="O14" s="2"/>
       <c r="Q14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1564,20 +1565,20 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H15" s="2">
         <v>7</v>
@@ -1586,10 +1587,10 @@
         <v>7</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1597,11 +1598,11 @@
       <c r="Q15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -1609,44 +1610,44 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="S16" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T16" s="2"/>
       <c r="U16" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1654,42 +1655,42 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M17" s="2"/>
       <c r="O17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -1697,28 +1698,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1726,13 +1727,13 @@
       <c r="Q18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -1740,20 +1741,20 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H19" s="2">
         <v>12</v>
@@ -1762,21 +1763,21 @@
         <v>12</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="O19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="S19" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T19" s="2"/>
       <c r="U19" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V19" s="2"/>
     </row>
@@ -1785,44 +1786,44 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -1830,40 +1831,40 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M21" s="2"/>
       <c r="O21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
@@ -1873,20 +1874,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H22" s="2">
         <v>23</v>
@@ -1895,28 +1896,28 @@
         <v>24</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="O22" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="S22" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -1924,31 +1925,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M23" s="2"/>
       <c r="O23" s="2"/>
@@ -1957,7 +1958,7 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -1965,44 +1966,44 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H24" s="2">
         <v>21</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M24" s="2"/>
       <c r="O24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U24" s="2"/>
       <c r="V24" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2010,30 +2011,30 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
         <v>21</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -2042,10 +2043,10 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -2053,44 +2054,44 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M26" s="2"/>
       <c r="O26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U26" s="2"/>
       <c r="V26" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2098,44 +2099,44 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M27" s="2"/>
       <c r="O27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -2143,39 +2144,39 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M28" s="2"/>
       <c r="O28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="S28" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
@@ -2186,20 +2187,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="H29" s="2">
         <v>29</v>
@@ -2208,17 +2209,17 @@
         <v>29</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="O29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="S29" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -2229,22 +2230,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="H30" s="2">
         <v>28</v>
@@ -2253,17 +2254,17 @@
         <v>28</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="O30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="S30" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -2274,37 +2275,37 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M31" s="2"/>
       <c r="O31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
@@ -2315,42 +2316,42 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M32" s="2"/>
       <c r="O32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="S32" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -2358,42 +2359,42 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="O33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="S33" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -2401,27 +2402,27 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M34" s="2"/>
       <c r="O34" s="2"/>
@@ -2429,10 +2430,10 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -2440,51 +2441,51 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S35" s="2"/>
       <c r="T35" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U35" s="2"/>
       <c r="V35" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -2492,46 +2493,46 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2">
         <v>37</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="O36" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="S36" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T36" s="2"/>
       <c r="U36" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -2539,20 +2540,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H37" s="2">
         <v>5</v>
@@ -2561,24 +2562,24 @@
         <v>5</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="O37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="S37" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U37" s="2"/>
       <c r="V37" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -2586,44 +2587,44 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
         <v>35</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="O38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="S38" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -2631,44 +2632,44 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M39" s="2"/>
       <c r="O39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="S39" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U39" s="2"/>
       <c r="V39" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -2676,42 +2677,42 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="O40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="S40" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -2719,44 +2720,44 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S41" s="2"/>
       <c r="T41" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
@@ -2766,33 +2767,33 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M42" s="2"/>
       <c r="O42" s="2"/>
@@ -2800,7 +2801,7 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V42" s="2"/>
     </row>
@@ -2809,31 +2810,31 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M43" s="2"/>
       <c r="O43" s="2"/>
@@ -2841,7 +2842,7 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V43" s="2"/>
     </row>
@@ -2850,28 +2851,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -2879,10 +2880,10 @@
       <c r="Q44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="V44" s="2"/>
     </row>

</xml_diff>

<commit_message>
Beta 0.9.1 - Expanded -selectr
</commit_message>
<xml_diff>
--- a/NTDS_Amsterdam.xlsx
+++ b/NTDS_Amsterdam.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15600" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="16800" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="164">
   <si>
     <t>E-mail</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Ja</t>
   </si>
   <si>
-    <t>Team-captain</t>
-  </si>
-  <si>
     <t>EHBO</t>
   </si>
   <si>
@@ -509,16 +506,16 @@
     <t>Jury Latin</t>
   </si>
   <si>
-    <t>Allergiën / dieet</t>
-  </si>
-  <si>
     <t>Wil je vrijwilliger zijn voor dit NTDS?</t>
   </si>
   <si>
     <t>Ben je op een eerder ETDS of NTDS vrijwilliger geweest?</t>
   </si>
   <si>
-    <t>Doe je mee aan de Same Seks wedstrijd?</t>
+    <t>Teamcaptain</t>
+  </si>
+  <si>
+    <t>Allergiën / Dieet</t>
   </si>
 </sst>
 </file>
@@ -882,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X72"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:X1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,18 +911,18 @@
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -937,16 +934,16 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -955,66 +952,63 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>5</v>
@@ -1028,36 +1022,36 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>5</v>
@@ -1071,30 +1065,30 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="2">
         <v>8</v>
@@ -1103,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="2"/>
@@ -1119,33 +1113,33 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1162,27 +1156,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H6" s="2">
         <v>36</v>
@@ -1191,10 +1185,10 @@
         <v>36</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1209,33 +1203,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>5</v>
@@ -1253,31 +1247,31 @@
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H8" s="2">
         <v>14</v>
@@ -1286,10 +1280,10 @@
         <v>14</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1304,25 +1298,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H9" s="2">
         <v>3</v>
@@ -1331,10 +1325,10 @@
         <v>3</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1347,35 +1341,35 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1384,37 +1378,37 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>5</v>
@@ -1431,33 +1425,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>5</v>
@@ -1476,28 +1470,28 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="2">
         <v>18</v>
@@ -1506,10 +1500,10 @@
         <v>18</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1524,28 +1518,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="2" t="s">
@@ -1563,28 +1557,28 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H15" s="2">
         <v>7</v>
@@ -1593,10 +1587,10 @@
         <v>7</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1611,38 +1605,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="S16" s="2" t="s">
@@ -1650,10 +1644,10 @@
       </c>
       <c r="T16" s="2"/>
       <c r="U16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1661,28 +1655,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>5</v>
@@ -1704,28 +1698,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1736,10 +1730,10 @@
         <v>5</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -1747,20 +1741,20 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H19" s="2">
         <v>12</v>
@@ -1769,10 +1763,10 @@
         <v>12</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1783,7 +1777,7 @@
       </c>
       <c r="T19" s="2"/>
       <c r="U19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V19" s="2"/>
     </row>
@@ -1792,33 +1786,33 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="S20" s="2" t="s">
@@ -1829,7 +1823,7 @@
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -1837,30 +1831,30 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>5</v>
@@ -1880,20 +1874,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H22" s="2">
         <v>23</v>
@@ -1902,15 +1896,15 @@
         <v>24</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="O22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="S22" s="2" t="s">
@@ -1920,7 +1914,7 @@
         <v>5</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V22" s="2" t="s">
         <v>5</v>
@@ -1931,28 +1925,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>5</v>
@@ -1964,7 +1958,7 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -1972,30 +1966,30 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H24" s="2">
         <v>21</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>5</v>
@@ -2009,7 +2003,7 @@
       </c>
       <c r="U24" s="2"/>
       <c r="V24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2017,30 +2011,30 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
         <v>21</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -2049,10 +2043,10 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -2060,30 +2054,30 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>5</v>
@@ -2097,7 +2091,7 @@
       </c>
       <c r="U26" s="2"/>
       <c r="V26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2105,28 +2099,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>5</v>
@@ -2139,7 +2133,7 @@
         <v>5</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V27" s="2" t="s">
         <v>5</v>
@@ -2150,30 +2144,30 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>5</v>
@@ -2193,20 +2187,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H29" s="2">
         <v>29</v>
@@ -2215,10 +2209,10 @@
         <v>29</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -2236,22 +2230,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H30" s="2">
         <v>28</v>
@@ -2260,10 +2254,10 @@
         <v>28</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2281,28 +2275,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>5</v>
@@ -2322,28 +2316,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>5</v>
@@ -2357,7 +2351,7 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -2365,28 +2359,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -2397,7 +2391,7 @@
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V33" s="2" t="s">
         <v>5</v>
@@ -2408,23 +2402,23 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="2" t="s">
@@ -2436,10 +2430,10 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -2447,37 +2441,37 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="F35" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>5</v>
@@ -2491,7 +2485,7 @@
       </c>
       <c r="U35" s="2"/>
       <c r="V35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -2499,35 +2493,35 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2">
         <v>37</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="O36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="S36" s="2" t="s">
@@ -2535,10 +2529,10 @@
       </c>
       <c r="T36" s="2"/>
       <c r="U36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -2546,20 +2540,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H37" s="2">
         <v>5</v>
@@ -2568,10 +2562,10 @@
         <v>5</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
@@ -2585,7 +2579,7 @@
       </c>
       <c r="U37" s="2"/>
       <c r="V37" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -2593,30 +2587,30 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2">
         <v>35</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -2627,10 +2621,10 @@
       </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -2638,28 +2632,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="F39" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>5</v>
@@ -2675,7 +2669,7 @@
       </c>
       <c r="U39" s="2"/>
       <c r="V39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -2683,30 +2677,30 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
@@ -2718,7 +2712,7 @@
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -2726,28 +2720,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>5</v>
@@ -2773,30 +2767,30 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>5</v>
@@ -2807,7 +2801,7 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V42" s="2"/>
     </row>
@@ -2816,28 +2810,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="F43" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>5</v>
@@ -2848,7 +2842,7 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V43" s="2"/>
     </row>
@@ -2857,28 +2851,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="F44" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -2889,7 +2883,7 @@
         <v>5</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V44" s="2"/>
     </row>

</xml_diff>

<commit_message>
Beta 0.9.9 - Signupsheet check done, bug fixes
</commit_message>
<xml_diff>
--- a/NTDS_Amsterdam.xlsx
+++ b/NTDS_Amsterdam.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="615" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="1815" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="164">
   <si>
     <t>Nr.</t>
   </si>
@@ -909,8 +909,8 @@
   <dimension ref="A1:W201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1258,7 +1258,9 @@
       <c r="L7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="M7" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1485,7 +1487,9 @@
       <c r="L12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="5"/>
+      <c r="M12" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O12" s="5" t="s">
         <v>29</v>
       </c>
@@ -2032,9 +2036,7 @@
       <c r="K24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="O24" s="5" t="s">
         <v>29</v>
@@ -2125,7 +2127,9 @@
       <c r="L26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M26" s="5"/>
+      <c r="M26" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O26" s="5" t="s">
         <v>29</v>
       </c>
@@ -2217,7 +2221,9 @@
       <c r="L28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M28" s="5"/>
+      <c r="M28" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O28" s="5"/>
       <c r="Q28" s="5"/>
       <c r="S28" s="5"/>
@@ -2521,7 +2527,9 @@
       <c r="L35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M35" s="5"/>
+      <c r="M35" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O35" s="5" t="s">
         <v>29</v>
       </c>
@@ -2804,7 +2812,9 @@
       <c r="L41" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M41" s="5"/>
+      <c r="M41" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="N41" s="2" t="s">
         <v>28</v>
       </c>
@@ -2854,7 +2864,9 @@
       <c r="L42" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M42" s="5"/>
+      <c r="M42" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="O42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="S42" s="5"/>
@@ -3844,7 +3856,7 @@
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="str">
-        <f t="shared" ref="A194:A225" si="6">IF(B194&lt;&gt;"",ROW(A194)-1,"")</f>
+        <f t="shared" ref="A194:A201" si="6">IF(B194&lt;&gt;"",ROW(A194)-1,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>